<commit_message>
PCB history and stuf, add fab files
</commit_message>
<xml_diff>
--- a/BOMs/BOM-full.xlsx
+++ b/BOMs/BOM-full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Fall-2022\Junior-Design\555-timer-PWM-fan\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6581B91E-DC9D-4753-80DA-1C600F6A5906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55104883-B74D-43B1-9330-4FE81B0C64BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Name/Desc</t>
   </si>
@@ -171,6 +171,33 @@
   </si>
   <si>
     <t>https://www.amazon.com/DYWISHKEY-Pieces-Stainless-Socket-Screws/dp/B07VPGQ1RZ/ref=sr_1_3?crid=XJIFUT6QS0ZK&amp;keywords=m3+screw+long&amp;qid=1662566283&amp;sprefix=m3+screw+long%2Caps%2C72&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power NMOS </t>
+  </si>
+  <si>
+    <t>LM395T/NOPB-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM395T-NOPB/8902</t>
+  </si>
+  <si>
+    <t>120VAC to 12VDC Converter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/ALITOVE-Converter-Cigarette-Transformer-Refrigerator/dp/B078RZQ9WY/</t>
+  </si>
+  <si>
+    <t>RCU-0C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test points </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/RCU-0C/2366048</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -272,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -291,6 +318,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,9 +673,9 @@
         <f>E2*F2</f>
         <v>16.95</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="7" t="e">
         <f>SUM(H2:H98)</f>
-        <v>27.959999999999997</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -668,7 +698,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="7">
-        <f t="shared" ref="H3:H16" si="0">E3*F3</f>
+        <f t="shared" ref="H3:H19" si="0">E3*F3</f>
         <v>8.1300000000000008</v>
       </c>
     </row>
@@ -709,9 +739,6 @@
       <c r="E5" s="8">
         <v>2</v>
       </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
       <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
@@ -733,9 +760,6 @@
       <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
       <c r="G6" s="8" t="s">
         <v>28</v>
       </c>
@@ -757,15 +781,15 @@
       <c r="E7" s="8">
         <v>3</v>
       </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H7" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -781,9 +805,6 @@
       <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
       <c r="G8" s="8" t="s">
         <v>28</v>
       </c>
@@ -805,9 +826,6 @@
       <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
       <c r="G9" s="8" t="s">
         <v>28</v>
       </c>
@@ -829,9 +847,6 @@
       <c r="E10" s="8">
         <v>1</v>
       </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
       <c r="G10" t="s">
         <v>33</v>
       </c>
@@ -853,9 +868,6 @@
       <c r="E11" s="8">
         <v>1</v>
       </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
       <c r="G11" s="9" t="s">
         <v>39</v>
       </c>
@@ -877,9 +889,6 @@
       <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
       <c r="G12" t="s">
         <v>35</v>
       </c>
@@ -901,9 +910,6 @@
       <c r="E13" s="8">
         <v>1</v>
       </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
       <c r="G13" t="s">
         <v>27</v>
       </c>
@@ -925,9 +931,6 @@
       <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
       <c r="G14" t="s">
         <v>44</v>
       </c>
@@ -949,9 +952,6 @@
       <c r="E15" s="8">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
       <c r="G15" s="8" t="s">
         <v>28</v>
       </c>
@@ -973,13 +973,73 @@
       <c r="E16" s="8">
         <v>4</v>
       </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
       <c r="G16" t="s">
         <v>42</v>
       </c>
       <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -988,8 +1048,9 @@
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{713DFAB9-46D0-41B2-842A-C74E4056294E}"/>
     <hyperlink ref="G11" r:id="rId2" xr:uid="{C63B6053-B37F-4B5A-B988-98B3AA898872}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{A1C9EFB6-F0DB-4D75-BDFF-D75079988624}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>